<commit_message>
convert ships: respect NotUsed flag
Former-commit-id: 165705d09b9c49e0ab4e3d08f85f58be067fd512 [formerly 4551389eb2e0b9d6eb95bc47a46a35aa9349beeb]
Former-commit-id: affbd664f741b4227ae1da9be0a74c0e38a8bd21
</commit_message>
<xml_diff>
--- a/src/data/port-battle.xlsx
+++ b/src/data/port-battle.xlsx
@@ -89,24 +89,24 @@
     <t>Wasa</t>
   </si>
   <si>
+    <t>Agamemnon</t>
+  </si>
+  <si>
+    <t>Rättvisan</t>
+  </si>
+  <si>
     <t>Leopard</t>
   </si>
   <si>
-    <t>Agamemnon</t>
-  </si>
-  <si>
-    <t>Rättvisan</t>
+    <t>Indefatigable</t>
+  </si>
+  <si>
+    <t>Ingermanland</t>
   </si>
   <si>
     <t>Wapen von Hamburg</t>
   </si>
   <si>
-    <t>Indefatigable</t>
-  </si>
-  <si>
-    <t>Ingermanland</t>
-  </si>
-  <si>
     <t>Endymion</t>
   </si>
   <si>
@@ -143,15 +143,15 @@
     <t>Le Gros Ventre Refit</t>
   </si>
   <si>
+    <t>La Renommée</t>
+  </si>
+  <si>
+    <t>Le Gros Ventre</t>
+  </si>
+  <si>
     <t>Surprise</t>
   </si>
   <si>
-    <t>La Renommée</t>
-  </si>
-  <si>
-    <t>Le Gros Ventre</t>
-  </si>
-  <si>
     <t>Hercules</t>
   </si>
   <si>
@@ -1103,19 +1103,19 @@
     <t>X</t>
   </si>
   <si>
+    <t>Prince de Neufchâtel</t>
+  </si>
+  <si>
     <t>Mercury</t>
   </si>
   <si>
+    <t>Navy Brig</t>
+  </si>
+  <si>
+    <t>Rattlesnake</t>
+  </si>
+  <si>
     <t>Snow</t>
-  </si>
-  <si>
-    <t>Prince de Neufchâtel</t>
-  </si>
-  <si>
-    <t>Navy Brig</t>
-  </si>
-  <si>
-    <t>Rattlesnake</t>
   </si>
   <si>
     <t>Brig</t>
@@ -1689,7 +1689,7 @@
         <v>54</v>
       </c>
       <c r="AF2" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="3" spans="1:32" customHeight="1">
@@ -1739,7 +1739,7 @@
         <v>55</v>
       </c>
       <c r="AF3" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="4" spans="1:32" customHeight="1">
@@ -1783,7 +1783,7 @@
         <v>56</v>
       </c>
       <c r="AF4" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="5" spans="1:32" customHeight="1">
@@ -1939,7 +1939,7 @@
         <v>59</v>
       </c>
       <c r="AF7" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="8" spans="1:32" customHeight="1">
@@ -1987,7 +1987,7 @@
         <v>60</v>
       </c>
       <c r="AF8" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="9" spans="1:32" customHeight="1">
@@ -2035,7 +2035,7 @@
         <v>61</v>
       </c>
       <c r="AF9" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="10" spans="1:32" customHeight="1">
@@ -2046,7 +2046,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="30" t="n">
-        <v>570</v>
+        <v>550</v>
       </c>
       <c r="D10" s="30">
         <f>COUNTA(F10:AD10)</f>
@@ -2131,7 +2131,7 @@
         <v>63</v>
       </c>
       <c r="AF11" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="12" spans="1:32" customHeight="1">
@@ -2179,7 +2179,7 @@
         <v>64</v>
       </c>
       <c r="AF12" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="13" spans="1:32" customHeight="1">
@@ -2227,7 +2227,7 @@
         <v>65</v>
       </c>
       <c r="AF13" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="14" spans="1:32" customHeight="1">
@@ -2275,7 +2275,7 @@
         <v>66</v>
       </c>
       <c r="AF14" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="15" spans="1:32" customHeight="1">
@@ -2323,7 +2323,7 @@
         <v>67</v>
       </c>
       <c r="AF15" s="0" t="n">
-        <v>20000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="16" spans="1:32" customHeight="1">
@@ -2419,7 +2419,7 @@
         <v>69</v>
       </c>
       <c r="AF17" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="18" spans="1:32" customHeight="1">
@@ -2430,7 +2430,7 @@
         <v>25</v>
       </c>
       <c r="C18" s="30" t="n">
-        <v>400</v>
+        <v>340</v>
       </c>
       <c r="D18" s="30">
         <f>COUNTA(F18:AD18)</f>
@@ -2515,7 +2515,7 @@
         <v>71</v>
       </c>
       <c r="AF19" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="20" spans="1:32" customHeight="1">
@@ -2526,7 +2526,7 @@
         <v>27</v>
       </c>
       <c r="C20" s="30" t="n">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="D20" s="30">
         <f>COUNTA(F20:AD20)</f>
@@ -2574,7 +2574,7 @@
         <v>28</v>
       </c>
       <c r="C21" s="30" t="n">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="D21" s="30">
         <f>COUNTA(F21:AD21)</f>
@@ -2622,7 +2622,7 @@
         <v>29</v>
       </c>
       <c r="C22" s="30" t="n">
-        <v>320</v>
+        <v>290</v>
       </c>
       <c r="D22" s="30">
         <f>COUNTA(F22:AD22)</f>
@@ -2659,7 +2659,7 @@
         <v>74</v>
       </c>
       <c r="AF22" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="23" spans="1:32" customHeight="1">
@@ -2670,7 +2670,7 @@
         <v>30</v>
       </c>
       <c r="C23" s="30" t="n">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="D23" s="30">
         <f>COUNTA(F23:AD23)</f>
@@ -2707,7 +2707,7 @@
         <v>75</v>
       </c>
       <c r="AF23" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="24" spans="1:32" customHeight="1">
@@ -2755,7 +2755,7 @@
         <v>76</v>
       </c>
       <c r="AF24" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="25" spans="1:32" customHeight="1">
@@ -2899,7 +2899,7 @@
         <v>79</v>
       </c>
       <c r="AF27" s="0" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="28" spans="1:32" customHeight="1">
@@ -3043,7 +3043,7 @@
         <v>82</v>
       </c>
       <c r="AF30" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="31" spans="1:32" customHeight="1">
@@ -3091,7 +3091,7 @@
         <v>83</v>
       </c>
       <c r="AF31" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="32" spans="1:32" customHeight="1">
@@ -3187,7 +3187,7 @@
         <v>85</v>
       </c>
       <c r="AF33" s="0" t="n">
-        <v>20000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="34" spans="1:32" customHeight="1">
@@ -3283,7 +3283,7 @@
         <v>87</v>
       </c>
       <c r="AF35" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="36" spans="1:32" customHeight="1">
@@ -3294,7 +3294,7 @@
         <v>43</v>
       </c>
       <c r="C36" s="26" t="n">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D36" s="26">
         <f>COUNTA(F36:AD36)</f>
@@ -3331,7 +3331,7 @@
         <v>88</v>
       </c>
       <c r="AF36" s="0" t="n">
-        <v>20000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="37" spans="1:32" customHeight="1">
@@ -3475,7 +3475,7 @@
         <v>91</v>
       </c>
       <c r="AF39" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="40" spans="1:32" customHeight="1">
@@ -3523,7 +3523,7 @@
         <v>92</v>
       </c>
       <c r="AF40" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="41" spans="1:32" customHeight="1">
@@ -3571,7 +3571,7 @@
         <v>93</v>
       </c>
       <c r="AF41" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="42" spans="1:32" customHeight="1">
@@ -3619,7 +3619,7 @@
         <v>94</v>
       </c>
       <c r="AF42" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="43" spans="1:32" customHeight="1">
@@ -3667,7 +3667,7 @@
         <v>95</v>
       </c>
       <c r="AF43" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="44" spans="1:32" customHeight="1">
@@ -3715,7 +3715,7 @@
         <v>96</v>
       </c>
       <c r="AF44" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="45" spans="1:32" customHeight="1">
@@ -3763,7 +3763,7 @@
         <v>97</v>
       </c>
       <c r="AF45" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="46" spans="31:32" customHeight="1">
@@ -3779,7 +3779,7 @@
         <v>99</v>
       </c>
       <c r="AF47" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="48" spans="31:32" customHeight="1">
@@ -3819,7 +3819,7 @@
         <v>104</v>
       </c>
       <c r="AF52" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="53" spans="31:32" customHeight="1">
@@ -3835,7 +3835,7 @@
         <v>106</v>
       </c>
       <c r="AF54" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="55" spans="31:32" customHeight="1">
@@ -3843,7 +3843,7 @@
         <v>107</v>
       </c>
       <c r="AF55" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="56" spans="31:32" customHeight="1">
@@ -3851,7 +3851,7 @@
         <v>108</v>
       </c>
       <c r="AF56" s="0" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="57" spans="31:32" customHeight="1">
@@ -3859,7 +3859,7 @@
         <v>109</v>
       </c>
       <c r="AF57" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="58" spans="31:32" customHeight="1">
@@ -3867,7 +3867,7 @@
         <v>110</v>
       </c>
       <c r="AF58" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="59" spans="31:32" customHeight="1">
@@ -3875,7 +3875,7 @@
         <v>111</v>
       </c>
       <c r="AF59" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="60" spans="31:32" customHeight="1">
@@ -3883,7 +3883,7 @@
         <v>112</v>
       </c>
       <c r="AF60" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="61" spans="31:32" customHeight="1">
@@ -3891,7 +3891,7 @@
         <v>113</v>
       </c>
       <c r="AF61" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="62" spans="31:32" customHeight="1">
@@ -3899,7 +3899,7 @@
         <v>114</v>
       </c>
       <c r="AF62" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="63" spans="31:32" customHeight="1">
@@ -3907,7 +3907,7 @@
         <v>115</v>
       </c>
       <c r="AF63" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="64" spans="31:32" customHeight="1">
@@ -3915,7 +3915,7 @@
         <v>116</v>
       </c>
       <c r="AF64" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="65" spans="31:32" customHeight="1">
@@ -3923,7 +3923,7 @@
         <v>117</v>
       </c>
       <c r="AF65" s="0" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="66" spans="31:32" customHeight="1">
@@ -3931,7 +3931,7 @@
         <v>118</v>
       </c>
       <c r="AF66" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="67" spans="31:32" customHeight="1">
@@ -3971,7 +3971,7 @@
         <v>123</v>
       </c>
       <c r="AF71" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="72" spans="31:32" customHeight="1">
@@ -3979,7 +3979,7 @@
         <v>124</v>
       </c>
       <c r="AF72" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="73" spans="31:32" customHeight="1">
@@ -3987,7 +3987,7 @@
         <v>125</v>
       </c>
       <c r="AF73" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="74" spans="31:32" customHeight="1">
@@ -3995,7 +3995,7 @@
         <v>126</v>
       </c>
       <c r="AF74" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="75" spans="31:32" customHeight="1">
@@ -4003,7 +4003,7 @@
         <v>127</v>
       </c>
       <c r="AF75" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="76" spans="31:32" customHeight="1">
@@ -4011,7 +4011,7 @@
         <v>128</v>
       </c>
       <c r="AF76" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="77" spans="31:32" customHeight="1">
@@ -4019,7 +4019,7 @@
         <v>129</v>
       </c>
       <c r="AF77" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="78" spans="31:32" customHeight="1">
@@ -4027,7 +4027,7 @@
         <v>130</v>
       </c>
       <c r="AF78" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="79" spans="31:32" customHeight="1">
@@ -4035,7 +4035,7 @@
         <v>131</v>
       </c>
       <c r="AF79" s="0" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="80" spans="31:32" customHeight="1">
@@ -4043,7 +4043,7 @@
         <v>132</v>
       </c>
       <c r="AF80" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="81" spans="31:32" customHeight="1">
@@ -4051,7 +4051,7 @@
         <v>133</v>
       </c>
       <c r="AF81" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="82" spans="31:32" customHeight="1">
@@ -4067,7 +4067,7 @@
         <v>135</v>
       </c>
       <c r="AF83" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="84" spans="31:32" customHeight="1">
@@ -4083,7 +4083,7 @@
         <v>137</v>
       </c>
       <c r="AF85" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="86" spans="31:32" customHeight="1">
@@ -4091,7 +4091,7 @@
         <v>138</v>
       </c>
       <c r="AF86" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="87" spans="31:32" customHeight="1">
@@ -4099,7 +4099,7 @@
         <v>139</v>
       </c>
       <c r="AF87" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="88" spans="31:32" customHeight="1">
@@ -4107,7 +4107,7 @@
         <v>140</v>
       </c>
       <c r="AF88" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="89" spans="31:32" customHeight="1">
@@ -4115,7 +4115,7 @@
         <v>141</v>
       </c>
       <c r="AF89" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="90" spans="31:32" customHeight="1">
@@ -4123,7 +4123,7 @@
         <v>142</v>
       </c>
       <c r="AF90" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="91" spans="31:32" customHeight="1">
@@ -4131,7 +4131,7 @@
         <v>143</v>
       </c>
       <c r="AF91" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="92" spans="31:32" customHeight="1">
@@ -4147,7 +4147,7 @@
         <v>145</v>
       </c>
       <c r="AF93" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="94" spans="31:32" customHeight="1">
@@ -4155,7 +4155,7 @@
         <v>146</v>
       </c>
       <c r="AF94" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="95" spans="31:32" customHeight="1">
@@ -4163,7 +4163,7 @@
         <v>147</v>
       </c>
       <c r="AF95" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="96" spans="31:32" customHeight="1">
@@ -4171,7 +4171,7 @@
         <v>148</v>
       </c>
       <c r="AF96" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="97" spans="31:32" customHeight="1">
@@ -4179,7 +4179,7 @@
         <v>149</v>
       </c>
       <c r="AF97" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="98" spans="31:32" customHeight="1">
@@ -4211,7 +4211,7 @@
         <v>153</v>
       </c>
       <c r="AF101" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="102" spans="31:32" customHeight="1">
@@ -4219,7 +4219,7 @@
         <v>154</v>
       </c>
       <c r="AF102" s="0" t="n">
-        <v>20000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="103" spans="31:32" customHeight="1">
@@ -4227,7 +4227,7 @@
         <v>155</v>
       </c>
       <c r="AF103" s="0" t="n">
-        <v>20000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="104" spans="31:32" customHeight="1">
@@ -4235,7 +4235,7 @@
         <v>156</v>
       </c>
       <c r="AF104" s="0" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="105" spans="31:32" customHeight="1">
@@ -4243,7 +4243,7 @@
         <v>157</v>
       </c>
       <c r="AF105" s="0" t="n">
-        <v>20000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="106" spans="31:32" customHeight="1">
@@ -4251,7 +4251,7 @@
         <v>158</v>
       </c>
       <c r="AF106" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="107" spans="31:32" customHeight="1">
@@ -4267,7 +4267,7 @@
         <v>160</v>
       </c>
       <c r="AF108" s="0" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="109" spans="31:32" customHeight="1">
@@ -4275,7 +4275,7 @@
         <v>161</v>
       </c>
       <c r="AF109" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="110" spans="31:32" customHeight="1">
@@ -4283,7 +4283,7 @@
         <v>162</v>
       </c>
       <c r="AF110" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="111" spans="31:32" customHeight="1">
@@ -4291,7 +4291,7 @@
         <v>163</v>
       </c>
       <c r="AF111" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="112" spans="31:32" customHeight="1">
@@ -4299,7 +4299,7 @@
         <v>164</v>
       </c>
       <c r="AF112" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="113" spans="31:32" customHeight="1">
@@ -4307,7 +4307,7 @@
         <v>165</v>
       </c>
       <c r="AF113" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="114" spans="31:32" customHeight="1">
@@ -4315,7 +4315,7 @@
         <v>166</v>
       </c>
       <c r="AF114" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="115" spans="31:32" customHeight="1">
@@ -4323,7 +4323,7 @@
         <v>167</v>
       </c>
       <c r="AF115" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="116" spans="31:32" customHeight="1">
@@ -4355,7 +4355,7 @@
         <v>171</v>
       </c>
       <c r="AF119" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="120" spans="31:32" customHeight="1">
@@ -4371,7 +4371,7 @@
         <v>173</v>
       </c>
       <c r="AF121" s="0" t="n">
-        <v>20000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="122" spans="31:32" customHeight="1">
@@ -4395,7 +4395,7 @@
         <v>176</v>
       </c>
       <c r="AF124" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="125" spans="31:32" customHeight="1">
@@ -4403,7 +4403,7 @@
         <v>177</v>
       </c>
       <c r="AF125" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="126" spans="31:32" customHeight="1">
@@ -4419,7 +4419,7 @@
         <v>179</v>
       </c>
       <c r="AF127" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="128" spans="31:32" customHeight="1">
@@ -4427,7 +4427,7 @@
         <v>180</v>
       </c>
       <c r="AF128" s="0" t="n">
-        <v>20000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="129" spans="31:32" customHeight="1">
@@ -4451,7 +4451,7 @@
         <v>183</v>
       </c>
       <c r="AF131" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="132" spans="31:32" customHeight="1">
@@ -4459,7 +4459,7 @@
         <v>184</v>
       </c>
       <c r="AF132" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="133" spans="31:32" customHeight="1">
@@ -4475,7 +4475,7 @@
         <v>186</v>
       </c>
       <c r="AF134" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="135" spans="31:32" customHeight="1">
@@ -4483,7 +4483,7 @@
         <v>187</v>
       </c>
       <c r="AF135" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="136" spans="31:32" customHeight="1">
@@ -4491,7 +4491,7 @@
         <v>188</v>
       </c>
       <c r="AF136" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="137" spans="31:32" customHeight="1">
@@ -4499,7 +4499,7 @@
         <v>189</v>
       </c>
       <c r="AF137" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="138" spans="31:32" customHeight="1">
@@ -4507,7 +4507,7 @@
         <v>190</v>
       </c>
       <c r="AF138" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="139" spans="31:32" customHeight="1">
@@ -4515,7 +4515,7 @@
         <v>191</v>
       </c>
       <c r="AF139" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="140" spans="31:32" customHeight="1">
@@ -4531,7 +4531,7 @@
         <v>193</v>
       </c>
       <c r="AF141" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="142" spans="31:32" customHeight="1">
@@ -4539,7 +4539,7 @@
         <v>194</v>
       </c>
       <c r="AF142" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="143" spans="31:32" customHeight="1">
@@ -4547,7 +4547,7 @@
         <v>195</v>
       </c>
       <c r="AF143" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="144" spans="31:32" customHeight="1">
@@ -4555,7 +4555,7 @@
         <v>196</v>
       </c>
       <c r="AF144" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="145" spans="31:32" customHeight="1">
@@ -4579,7 +4579,7 @@
         <v>199</v>
       </c>
       <c r="AF147" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="148" spans="31:32" customHeight="1">
@@ -4587,7 +4587,7 @@
         <v>200</v>
       </c>
       <c r="AF148" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="149" spans="31:32" customHeight="1">
@@ -4595,7 +4595,7 @@
         <v>201</v>
       </c>
       <c r="AF149" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="150" spans="31:32" customHeight="1">
@@ -4603,7 +4603,7 @@
         <v>202</v>
       </c>
       <c r="AF150" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="151" spans="31:32" customHeight="1">
@@ -4627,7 +4627,7 @@
         <v>205</v>
       </c>
       <c r="AF153" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="154" spans="31:32" customHeight="1">
@@ -4635,7 +4635,7 @@
         <v>206</v>
       </c>
       <c r="AF154" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="155" spans="31:32" customHeight="1">
@@ -4643,7 +4643,7 @@
         <v>207</v>
       </c>
       <c r="AF155" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="156" spans="31:32" customHeight="1">
@@ -4659,7 +4659,7 @@
         <v>209</v>
       </c>
       <c r="AF157" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="158" spans="31:32" customHeight="1">
@@ -4675,7 +4675,7 @@
         <v>211</v>
       </c>
       <c r="AF159" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="160" spans="31:32" customHeight="1">
@@ -4691,7 +4691,7 @@
         <v>213</v>
       </c>
       <c r="AF161" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="162" spans="31:32" customHeight="1">
@@ -4699,7 +4699,7 @@
         <v>214</v>
       </c>
       <c r="AF162" s="0" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="163" spans="31:32" customHeight="1">
@@ -4707,7 +4707,7 @@
         <v>215</v>
       </c>
       <c r="AF163" s="0" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="164" spans="31:32" customHeight="1">
@@ -4715,7 +4715,7 @@
         <v>216</v>
       </c>
       <c r="AF164" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="165" spans="31:32" customHeight="1">
@@ -4723,7 +4723,7 @@
         <v>217</v>
       </c>
       <c r="AF165" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="166" spans="31:32" customHeight="1">
@@ -4747,7 +4747,7 @@
         <v>220</v>
       </c>
       <c r="AF168" s="0" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="169" spans="31:32" customHeight="1">
@@ -4755,7 +4755,7 @@
         <v>221</v>
       </c>
       <c r="AF169" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="170" spans="31:32" customHeight="1">
@@ -4763,7 +4763,7 @@
         <v>222</v>
       </c>
       <c r="AF170" s="0" t="n">
-        <v>20000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="171" spans="31:32" customHeight="1">
@@ -4771,7 +4771,7 @@
         <v>223</v>
       </c>
       <c r="AF171" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="172" spans="31:32" customHeight="1">
@@ -4779,7 +4779,7 @@
         <v>224</v>
       </c>
       <c r="AF172" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="173" spans="31:32" customHeight="1">
@@ -4787,7 +4787,7 @@
         <v>225</v>
       </c>
       <c r="AF173" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="174" spans="31:32" customHeight="1">
@@ -4795,7 +4795,7 @@
         <v>226</v>
       </c>
       <c r="AF174" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="175" spans="31:32" customHeight="1">
@@ -4803,7 +4803,7 @@
         <v>227</v>
       </c>
       <c r="AF175" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="176" spans="31:32" customHeight="1">
@@ -4811,7 +4811,7 @@
         <v>228</v>
       </c>
       <c r="AF176" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="177" spans="31:32" customHeight="1">
@@ -4819,7 +4819,7 @@
         <v>229</v>
       </c>
       <c r="AF177" s="0" t="n">
-        <v>25000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="178" spans="31:32" customHeight="1">
@@ -4827,7 +4827,7 @@
         <v>230</v>
       </c>
       <c r="AF178" s="0" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="179" spans="31:32" customHeight="1">
@@ -4843,7 +4843,7 @@
         <v>232</v>
       </c>
       <c r="AF180" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="181" spans="31:32" customHeight="1">
@@ -4851,7 +4851,7 @@
         <v>233</v>
       </c>
       <c r="AF181" s="0" t="n">
-        <v>20000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="182" spans="31:32" customHeight="1">
@@ -4859,7 +4859,7 @@
         <v>234</v>
       </c>
       <c r="AF182" s="0" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="183" spans="31:32" customHeight="1">
@@ -4875,7 +4875,7 @@
         <v>236</v>
       </c>
       <c r="AF184" s="0" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="185" spans="31:32" customHeight="1">
@@ -4883,7 +4883,7 @@
         <v>237</v>
       </c>
       <c r="AF185" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="186" spans="31:32" customHeight="1">
@@ -4891,7 +4891,7 @@
         <v>238</v>
       </c>
       <c r="AF186" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="187" spans="31:32" customHeight="1">
@@ -4899,7 +4899,7 @@
         <v>239</v>
       </c>
       <c r="AF187" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="188" spans="31:32" customHeight="1">
@@ -4907,7 +4907,7 @@
         <v>240</v>
       </c>
       <c r="AF188" s="0" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="189" spans="31:32" customHeight="1">
@@ -4915,7 +4915,7 @@
         <v>241</v>
       </c>
       <c r="AF189" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="190" spans="31:32" customHeight="1">
@@ -4931,7 +4931,7 @@
         <v>243</v>
       </c>
       <c r="AF191" s="0" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="192" spans="31:32" customHeight="1">
@@ -4939,7 +4939,7 @@
         <v>244</v>
       </c>
       <c r="AF192" s="0" t="n">
-        <v>20000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="193" spans="31:32" customHeight="1">
@@ -4947,7 +4947,7 @@
         <v>245</v>
       </c>
       <c r="AF193" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="194" spans="31:32" customHeight="1">
@@ -4955,7 +4955,7 @@
         <v>246</v>
       </c>
       <c r="AF194" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="195" spans="31:32" customHeight="1">
@@ -4963,7 +4963,7 @@
         <v>247</v>
       </c>
       <c r="AF195" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="196" spans="31:32" customHeight="1">
@@ -4971,7 +4971,7 @@
         <v>248</v>
       </c>
       <c r="AF196" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="197" spans="31:32" customHeight="1">
@@ -4979,7 +4979,7 @@
         <v>249</v>
       </c>
       <c r="AF197" s="0" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="198" spans="31:32" customHeight="1">
@@ -4987,7 +4987,7 @@
         <v>250</v>
       </c>
       <c r="AF198" s="0" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="199" spans="31:32" customHeight="1">
@@ -5035,7 +5035,7 @@
         <v>256</v>
       </c>
       <c r="AF204" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="205" spans="31:32" customHeight="1">
@@ -5051,7 +5051,7 @@
         <v>258</v>
       </c>
       <c r="AF206" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="207" spans="31:32" customHeight="1">
@@ -5067,7 +5067,7 @@
         <v>260</v>
       </c>
       <c r="AF208" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="209" spans="31:32" customHeight="1">
@@ -5083,7 +5083,7 @@
         <v>262</v>
       </c>
       <c r="AF210" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="211" spans="31:32" customHeight="1">
@@ -5107,7 +5107,7 @@
         <v>265</v>
       </c>
       <c r="AF213" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="214" spans="31:32" customHeight="1">
@@ -5115,7 +5115,7 @@
         <v>266</v>
       </c>
       <c r="AF214" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="215" spans="31:32" customHeight="1">
@@ -5131,7 +5131,7 @@
         <v>268</v>
       </c>
       <c r="AF216" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="217" spans="31:32" customHeight="1">
@@ -5147,7 +5147,7 @@
         <v>270</v>
       </c>
       <c r="AF218" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="219" spans="31:32" customHeight="1">
@@ -5163,7 +5163,7 @@
         <v>272</v>
       </c>
       <c r="AF220" s="0" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="221" spans="31:32" customHeight="1">
@@ -5171,7 +5171,7 @@
         <v>273</v>
       </c>
       <c r="AF221" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="222" spans="31:32" customHeight="1">
@@ -5187,7 +5187,7 @@
         <v>275</v>
       </c>
       <c r="AF223" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="224" spans="31:32" customHeight="1">
@@ -5195,7 +5195,7 @@
         <v>276</v>
       </c>
       <c r="AF224" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="225" spans="31:32" customHeight="1">
@@ -5203,7 +5203,7 @@
         <v>277</v>
       </c>
       <c r="AF225" s="0" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="226" spans="31:32" customHeight="1">
@@ -5211,7 +5211,7 @@
         <v>278</v>
       </c>
       <c r="AF226" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="227" spans="31:32" customHeight="1">
@@ -5219,7 +5219,7 @@
         <v>279</v>
       </c>
       <c r="AF227" s="0" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="228" spans="31:32" customHeight="1">
@@ -5251,7 +5251,7 @@
         <v>283</v>
       </c>
       <c r="AF231" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="232" spans="31:32" customHeight="1">
@@ -5259,7 +5259,7 @@
         <v>284</v>
       </c>
       <c r="AF232" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="233" spans="31:32" customHeight="1">
@@ -5267,7 +5267,7 @@
         <v>285</v>
       </c>
       <c r="AF233" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="234" spans="31:32" customHeight="1">
@@ -5283,7 +5283,7 @@
         <v>287</v>
       </c>
       <c r="AF235" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="236" spans="31:32" customHeight="1">
@@ -5307,7 +5307,7 @@
         <v>290</v>
       </c>
       <c r="AF238" s="0" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="239" spans="31:32" customHeight="1">
@@ -5323,7 +5323,7 @@
         <v>292</v>
       </c>
       <c r="AF240" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="241" spans="31:32" customHeight="1">
@@ -5331,7 +5331,7 @@
         <v>293</v>
       </c>
       <c r="AF241" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="242" spans="31:32" customHeight="1">
@@ -5355,7 +5355,7 @@
         <v>296</v>
       </c>
       <c r="AF244" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="245" spans="31:32" customHeight="1">
@@ -5363,7 +5363,7 @@
         <v>297</v>
       </c>
       <c r="AF245" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="246" spans="31:32" customHeight="1">
@@ -5371,7 +5371,7 @@
         <v>298</v>
       </c>
       <c r="AF246" s="0" t="n">
-        <v>25000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="247" spans="31:32" customHeight="1">
@@ -5387,7 +5387,7 @@
         <v>300</v>
       </c>
       <c r="AF248" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="249" spans="31:32" customHeight="1">
@@ -5395,7 +5395,7 @@
         <v>301</v>
       </c>
       <c r="AF249" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="250" spans="31:32" customHeight="1">
@@ -5403,7 +5403,7 @@
         <v>302</v>
       </c>
       <c r="AF250" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="251" spans="31:32" customHeight="1">
@@ -5411,7 +5411,7 @@
         <v>303</v>
       </c>
       <c r="AF251" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="252" spans="31:32" customHeight="1">
@@ -5419,7 +5419,7 @@
         <v>304</v>
       </c>
       <c r="AF252" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="253" spans="31:32" customHeight="1">
@@ -5435,7 +5435,7 @@
         <v>306</v>
       </c>
       <c r="AF254" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="255" spans="31:32" customHeight="1">
@@ -5443,7 +5443,7 @@
         <v>307</v>
       </c>
       <c r="AF255" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="256" spans="31:32" customHeight="1">
@@ -5451,7 +5451,7 @@
         <v>308</v>
       </c>
       <c r="AF256" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="257" spans="31:32" customHeight="1">
@@ -5459,7 +5459,7 @@
         <v>309</v>
       </c>
       <c r="AF257" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="258" spans="31:32" customHeight="1">
@@ -5475,7 +5475,7 @@
         <v>311</v>
       </c>
       <c r="AF259" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="260" spans="31:32" customHeight="1">
@@ -5483,7 +5483,7 @@
         <v>312</v>
       </c>
       <c r="AF260" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="261" spans="31:32" customHeight="1">
@@ -5491,7 +5491,7 @@
         <v>313</v>
       </c>
       <c r="AF261" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="262" spans="31:32" customHeight="1">
@@ -5499,7 +5499,7 @@
         <v>314</v>
       </c>
       <c r="AF262" s="0" t="n">
-        <v>25000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="263" spans="31:32" customHeight="1">
@@ -5507,7 +5507,7 @@
         <v>315</v>
       </c>
       <c r="AF263" s="0" t="n">
-        <v>25000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="264" spans="31:32" customHeight="1">
@@ -5531,7 +5531,7 @@
         <v>318</v>
       </c>
       <c r="AF266" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="267" spans="31:32" customHeight="1">
@@ -5547,7 +5547,7 @@
         <v>320</v>
       </c>
       <c r="AF268" s="0" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="269" spans="31:32" customHeight="1">
@@ -5555,7 +5555,7 @@
         <v>321</v>
       </c>
       <c r="AF269" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="270" spans="31:32" customHeight="1">
@@ -5571,7 +5571,7 @@
         <v>323</v>
       </c>
       <c r="AF271" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="272" spans="31:32" customHeight="1">
@@ -5587,7 +5587,7 @@
         <v>325</v>
       </c>
       <c r="AF273" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="274" spans="31:32" customHeight="1">
@@ -5595,7 +5595,7 @@
         <v>326</v>
       </c>
       <c r="AF274" s="0" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="275" spans="31:32" customHeight="1">
@@ -5603,7 +5603,7 @@
         <v>327</v>
       </c>
       <c r="AF275" s="0" t="n">
-        <v>20000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="276" spans="31:32" customHeight="1">
@@ -5619,7 +5619,7 @@
         <v>329</v>
       </c>
       <c r="AF277" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="278" spans="31:32" customHeight="1">
@@ -5627,7 +5627,7 @@
         <v>330</v>
       </c>
       <c r="AF278" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="279" spans="31:32" customHeight="1">
@@ -5635,7 +5635,7 @@
         <v>331</v>
       </c>
       <c r="AF279" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="280" spans="31:32" customHeight="1">
@@ -5643,7 +5643,7 @@
         <v>332</v>
       </c>
       <c r="AF280" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="281" spans="31:32" customHeight="1">
@@ -5659,7 +5659,7 @@
         <v>334</v>
       </c>
       <c r="AF282" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="283" spans="31:32" customHeight="1">
@@ -5667,7 +5667,7 @@
         <v>335</v>
       </c>
       <c r="AF283" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="284" spans="31:32" customHeight="1">
@@ -5675,7 +5675,7 @@
         <v>336</v>
       </c>
       <c r="AF284" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="285" spans="31:32" customHeight="1">
@@ -5691,7 +5691,7 @@
         <v>338</v>
       </c>
       <c r="AF286" s="0" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="287" spans="31:32" customHeight="1">
@@ -5699,7 +5699,7 @@
         <v>339</v>
       </c>
       <c r="AF287" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="288" spans="31:32" customHeight="1">
@@ -5723,7 +5723,7 @@
         <v>342</v>
       </c>
       <c r="AF290" s="0" t="n">
-        <v>10000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="291" spans="31:32" customHeight="1">
@@ -5731,7 +5731,7 @@
         <v>343</v>
       </c>
       <c r="AF291" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="292" spans="31:32" customHeight="1">
@@ -5739,7 +5739,7 @@
         <v>344</v>
       </c>
       <c r="AF292" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="293" spans="31:32" customHeight="1">
@@ -5747,7 +5747,7 @@
         <v>345</v>
       </c>
       <c r="AF293" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="294" spans="31:32" customHeight="1">
@@ -5763,7 +5763,7 @@
         <v>347</v>
       </c>
       <c r="AF295" s="0" t="n">
-        <v>25000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="296" spans="31:32" customHeight="1">
@@ -5771,7 +5771,7 @@
         <v>348</v>
       </c>
       <c r="AF296" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="297" spans="31:32" customHeight="1">
@@ -5779,7 +5779,7 @@
         <v>349</v>
       </c>
       <c r="AF297" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="298" spans="31:32" customHeight="1">
@@ -5787,7 +5787,7 @@
         <v>350</v>
       </c>
       <c r="AF298" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="299" spans="31:32" customHeight="1">
@@ -5803,7 +5803,7 @@
         <v>352</v>
       </c>
       <c r="AF300" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="301" spans="31:32" customHeight="1">
@@ -5827,7 +5827,7 @@
         <v>355</v>
       </c>
       <c r="AF303" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="304" spans="31:32" customHeight="1">
@@ -5835,7 +5835,7 @@
         <v>356</v>
       </c>
       <c r="AF304" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="305" spans="31:32" customHeight="1">
@@ -5954,7 +5954,7 @@
         <v>376</v>
       </c>
       <c r="AF1" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="2" spans="1:32" customHeight="1">
@@ -6000,7 +6000,7 @@
         <v>377</v>
       </c>
       <c r="AF2" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="3" spans="1:32" customHeight="1">
@@ -6050,7 +6050,7 @@
         <v>378</v>
       </c>
       <c r="AF3" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="4" spans="1:32" customHeight="1">
@@ -6094,7 +6094,7 @@
         <v>379</v>
       </c>
       <c r="AF4" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="5" spans="1:32" customHeight="1">
@@ -6148,7 +6148,7 @@
         <v>380</v>
       </c>
       <c r="AF5" s="0" t="n">
-        <v>2500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="6" spans="1:32" customHeight="1">
@@ -6159,7 +6159,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="26" t="n">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D6" s="26">
         <f>COUNTA(F6:AD6)</f>
@@ -6202,7 +6202,7 @@
         <v>381</v>
       </c>
       <c r="AF6" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="7" spans="1:32" customHeight="1">
@@ -6210,7 +6210,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C7" s="26" t="n">
         <v>120</v>
@@ -6250,7 +6250,7 @@
         <v>382</v>
       </c>
       <c r="AF7" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="8" spans="1:32" customHeight="1">
@@ -6298,7 +6298,7 @@
         <v>383</v>
       </c>
       <c r="AF8" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="9" spans="1:32" customHeight="1">
@@ -6346,7 +6346,7 @@
         <v>384</v>
       </c>
       <c r="AF9" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="10" spans="1:32" customHeight="1">
@@ -6394,7 +6394,7 @@
         <v>385</v>
       </c>
       <c r="AF10" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="11" spans="1:32" customHeight="1">
@@ -6442,7 +6442,7 @@
         <v>386</v>
       </c>
       <c r="AF11" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="12" spans="1:32" customHeight="1">
@@ -6490,7 +6490,7 @@
         <v>387</v>
       </c>
       <c r="AF12" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="13" spans="1:32" customHeight="1">
@@ -6538,7 +6538,7 @@
         <v>388</v>
       </c>
       <c r="AF13" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="14" spans="1:32" customHeight="1">
@@ -6549,7 +6549,7 @@
         <v>363</v>
       </c>
       <c r="C14" s="30" t="n">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D14" s="30">
         <f>COUNTA(F14:AD14)</f>
@@ -6586,7 +6586,7 @@
         <v>389</v>
       </c>
       <c r="AF14" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="15" spans="1:32" customHeight="1">
@@ -6597,7 +6597,7 @@
         <v>364</v>
       </c>
       <c r="C15" s="30" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D15" s="30">
         <f>COUNTA(F15:AD15)</f>
@@ -6634,7 +6634,7 @@
         <v>390</v>
       </c>
       <c r="AF15" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="16" spans="1:32" customHeight="1">
@@ -6645,7 +6645,7 @@
         <v>365</v>
       </c>
       <c r="C16" s="30" t="n">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D16" s="30">
         <f>COUNTA(F16:AD16)</f>
@@ -6682,7 +6682,7 @@
         <v>391</v>
       </c>
       <c r="AF16" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="17" spans="1:32" customHeight="1">
@@ -6730,7 +6730,7 @@
         <v>392</v>
       </c>
       <c r="AF17" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="18" spans="1:32" customHeight="1">
@@ -6778,7 +6778,7 @@
         <v>393</v>
       </c>
       <c r="AF18" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="19" spans="1:32" customHeight="1">
@@ -6826,7 +6826,7 @@
         <v>394</v>
       </c>
       <c r="AF19" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="20" spans="1:32" customHeight="1">
@@ -6874,7 +6874,7 @@
         <v>395</v>
       </c>
       <c r="AF20" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="21" spans="1:32" customHeight="1">
@@ -6922,7 +6922,7 @@
         <v>396</v>
       </c>
       <c r="AF21" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="22" spans="1:32" customHeight="1">
@@ -6970,7 +6970,7 @@
         <v>397</v>
       </c>
       <c r="AF22" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="23" spans="1:32" customHeight="1">
@@ -7018,7 +7018,7 @@
         <v>398</v>
       </c>
       <c r="AF23" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="24" spans="1:32" customHeight="1">
@@ -7066,7 +7066,7 @@
         <v>399</v>
       </c>
       <c r="AF24" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="25" spans="1:32" customHeight="1">
@@ -7114,7 +7114,7 @@
         <v>400</v>
       </c>
       <c r="AF25" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="26" spans="1:32" customHeight="1">
@@ -7162,7 +7162,7 @@
         <v>401</v>
       </c>
       <c r="AF26" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="27" spans="31:32" customHeight="1">
@@ -7170,7 +7170,7 @@
         <v>402</v>
       </c>
       <c r="AF27" s="0" t="n">
-        <v>2500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="28" spans="31:32" customHeight="1">
@@ -7178,7 +7178,7 @@
         <v>403</v>
       </c>
       <c r="AF28" s="0" t="n">
-        <v>1500</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="29" spans="31:32" customHeight="1">
@@ -7186,7 +7186,7 @@
         <v>404</v>
       </c>
       <c r="AF29" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="30" spans="31:32" customHeight="1">
@@ -7194,7 +7194,7 @@
         <v>405</v>
       </c>
       <c r="AF30" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="31" spans="31:32" customHeight="1">
@@ -7202,7 +7202,7 @@
         <v>406</v>
       </c>
       <c r="AF31" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="32" spans="31:32" customHeight="1">
@@ -7210,7 +7210,7 @@
         <v>407</v>
       </c>
       <c r="AF32" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="33" spans="31:32" customHeight="1">
@@ -7218,7 +7218,7 @@
         <v>408</v>
       </c>
       <c r="AF33" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="34" spans="31:32" customHeight="1">
@@ -7226,7 +7226,7 @@
         <v>409</v>
       </c>
       <c r="AF34" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="35" spans="31:32" customHeight="1">
@@ -7234,7 +7234,7 @@
         <v>410</v>
       </c>
       <c r="AF35" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="36" spans="31:32" customHeight="1">
@@ -7242,7 +7242,7 @@
         <v>411</v>
       </c>
       <c r="AF36" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="37" spans="31:32" customHeight="1">
@@ -7250,7 +7250,7 @@
         <v>412</v>
       </c>
       <c r="AF37" s="0" t="n">
-        <v>2500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="38" spans="31:32" customHeight="1">
@@ -7258,7 +7258,7 @@
         <v>413</v>
       </c>
       <c r="AF38" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="39" spans="31:32" customHeight="1">
@@ -7266,7 +7266,7 @@
         <v>414</v>
       </c>
       <c r="AF39" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="40" spans="31:32" customHeight="1">
@@ -7274,7 +7274,7 @@
         <v>415</v>
       </c>
       <c r="AF40" s="0" t="n">
-        <v>1500</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="41" spans="31:32" customHeight="1">
@@ -7282,7 +7282,7 @@
         <v>416</v>
       </c>
       <c r="AF41" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="42" spans="31:32" customHeight="1">
@@ -7290,7 +7290,7 @@
         <v>417</v>
       </c>
       <c r="AF42" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="43" spans="31:32" customHeight="1">
@@ -7298,7 +7298,7 @@
         <v>418</v>
       </c>
       <c r="AF43" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="44" spans="31:32" customHeight="1">
@@ -7306,7 +7306,7 @@
         <v>419</v>
       </c>
       <c r="AF44" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="45" spans="31:32" customHeight="1">
@@ -7314,7 +7314,7 @@
         <v>420</v>
       </c>
       <c r="AF45" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="46" spans="31:32" customHeight="1">
@@ -7322,7 +7322,7 @@
         <v>421</v>
       </c>
       <c r="AF46" s="0" t="n">
-        <v>2500</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="47" spans="31:32" customHeight="1">
@@ -7330,7 +7330,7 @@
         <v>422</v>
       </c>
       <c r="AF47" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="48" spans="31:32" customHeight="1">
@@ -7338,7 +7338,7 @@
         <v>423</v>
       </c>
       <c r="AF48" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="49" spans="31:32" customHeight="1">
@@ -7346,7 +7346,7 @@
         <v>424</v>
       </c>
       <c r="AF49" s="0" t="n">
-        <v>2500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="50" spans="31:32" customHeight="1">
@@ -7354,7 +7354,7 @@
         <v>425</v>
       </c>
       <c r="AF50" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="51" spans="31:32" customHeight="1">
@@ -7362,7 +7362,7 @@
         <v>426</v>
       </c>
       <c r="AF51" s="0" t="n">
-        <v>3000</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="52" spans="31:32" customHeight="1">
@@ -7370,7 +7370,7 @@
         <v>427</v>
       </c>
       <c r="AF52" s="0" t="n">
-        <v>2500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="53" spans="31:32" customHeight="1">
@@ -7378,7 +7378,7 @@
         <v>428</v>
       </c>
       <c r="AF53" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="54" spans="31:32" customHeight="1">
@@ -7386,7 +7386,7 @@
         <v>429</v>
       </c>
       <c r="AF54" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="55" spans="31:32" customHeight="1">
@@ -7394,7 +7394,7 @@
         <v>430</v>
       </c>
       <c r="AF55" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="56" spans="31:32" customHeight="1">
@@ -7402,7 +7402,7 @@
         <v>431</v>
       </c>
       <c r="AF56" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="57" spans="31:32" customHeight="1">
@@ -7410,7 +7410,7 @@
         <v>432</v>
       </c>
       <c r="AF57" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="58" spans="31:32" customHeight="1">
@@ -7418,7 +7418,7 @@
         <v>433</v>
       </c>
       <c r="AF58" s="0" t="n">
-        <v>1500</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="59" spans="31:32" customHeight="1">
@@ -7426,7 +7426,7 @@
         <v>434</v>
       </c>
       <c r="AF59" s="0" t="n">
-        <v>2500</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="60" spans="31:32" customHeight="1">
@@ -7434,7 +7434,7 @@
         <v>435</v>
       </c>
       <c r="AF60" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="61" spans="31:32" customHeight="1">
@@ -7442,7 +7442,7 @@
         <v>436</v>
       </c>
       <c r="AF61" s="0" t="n">
-        <v>2500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="62" spans="31:32" customHeight="1">
@@ -7450,7 +7450,7 @@
         <v>437</v>
       </c>
       <c r="AF62" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="63" spans="31:32" customHeight="1">
@@ -7458,7 +7458,7 @@
         <v>438</v>
       </c>
       <c r="AF63" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="64" spans="31:32" customHeight="1">
@@ -7466,7 +7466,7 @@
         <v>439</v>
       </c>
       <c r="AF64" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="65" spans="31:32" customHeight="1">
@@ -7474,7 +7474,7 @@
         <v>440</v>
       </c>
       <c r="AF65" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="66" spans="31:32" customHeight="1">
@@ -7482,7 +7482,7 @@
         <v>441</v>
       </c>
       <c r="AF66" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="67" spans="31:32" customHeight="1">
@@ -7490,7 +7490,7 @@
         <v>442</v>
       </c>
       <c r="AF67" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="68" spans="31:32" customHeight="1">
@@ -7498,7 +7498,7 @@
         <v>443</v>
       </c>
       <c r="AF68" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="69" spans="31:32" customHeight="1">
@@ -7506,7 +7506,7 @@
         <v>444</v>
       </c>
       <c r="AF69" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="70" spans="31:32" customHeight="1">
@@ -7514,7 +7514,7 @@
         <v>445</v>
       </c>
       <c r="AF70" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="71" spans="31:32" customHeight="1">
@@ -7522,7 +7522,7 @@
         <v>446</v>
       </c>
       <c r="AF71" s="0" t="n">
-        <v>2500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="72" spans="31:32" customHeight="1">
@@ -7530,7 +7530,7 @@
         <v>447</v>
       </c>
       <c r="AF72" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="73" spans="31:32" customHeight="1">
@@ -7538,7 +7538,7 @@
         <v>448</v>
       </c>
       <c r="AF73" s="0" t="n">
-        <v>1500</v>
+        <v>900</v>
       </c>
     </row>
   </sheetData>

</xml_diff>